<commit_message>
Uploaded 16-Feb-2017 16:06:03 {/bonus-program/src/main/resources/dtables/bonus_program/bonus-program.xlsx}
</commit_message>
<xml_diff>
--- a/bonus-program/src/main/resources/dtables/bonus_program/bonus-program.xlsx
+++ b/bonus-program/src/main/resources/dtables/bonus_program/bonus-program.xlsx
@@ -12,7 +12,7 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="ClaimTypes" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" name="Excel_BuiltIn__FilterDatabase_1" vbProcedure="false">Tables!$G$10:$G$21</definedName>
+    <definedName function="false" hidden="false" name="Excel_BuiltIn__FilterDatabase_1" vbProcedure="false">Tables!$E$10:$E$21</definedName>
     <definedName function="false" hidden="false" name="Excel_BuiltIn__FilterDatabase_2" vbProcedure="false">#REF!</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -116,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>RuleSet</t>
   </si>
@@ -142,9 +142,6 @@
     <t>$e : Employee</t>
   </si>
   <si>
-    <t>$bonus : Bonus</t>
-  </si>
-  <si>
     <t>not Bonus</t>
   </si>
   <si>
@@ -154,16 +151,10 @@
     <t>yearsOfService &gt; $param</t>
   </si>
   <si>
-    <t>bigAbsence == $param</t>
-  </si>
-  <si>
     <t>employee == $param</t>
   </si>
   <si>
     <t>Bonus $b = new Bonus(); $b.setAmount((double)$param); $b.setEmployee($e); insert($b);</t>
-  </si>
-  <si>
-    <t>retract($param)</t>
   </si>
   <si>
     <t>Bonus rules</t>
@@ -175,19 +166,10 @@
     <t>Served more</t>
   </si>
   <si>
-    <t>absence</t>
-  </si>
-  <si>
-    <t>bonus for employee</t>
-  </si>
-  <si>
     <t>no bonus for employee</t>
   </si>
   <si>
     <t>Inser bonus of amount</t>
-  </si>
-  <si>
-    <t>retract</t>
   </si>
   <si>
     <t>Lowest bonus</t>
@@ -207,18 +189,14 @@
   <si>
     <t>High bonus</t>
   </si>
-  <si>
-    <t>$bonus</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -354,7 +332,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -455,10 +433,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -480,7 +454,7 @@
   <dimension ref="1:34"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -488,16 +462,16 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="0.13265306122449"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.8112244897959"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="7" min="4" style="1" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="30.6428571428571"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="1021" min="13" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -508,9 +482,9 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
+      <c r="H1" s="0"/>
+      <c r="I1" s="0"/>
+      <c r="J1" s="0"/>
       <c r="K1" s="0"/>
       <c r="L1" s="0"/>
       <c r="M1" s="0"/>
@@ -1522,9 +1496,6 @@
       <c r="AME1" s="0"/>
       <c r="AMF1" s="0"/>
       <c r="AMG1" s="0"/>
-      <c r="AMH1" s="0"/>
-      <c r="AMI1" s="0"/>
-      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A2" s="0"/>
@@ -1537,14 +1508,14 @@
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="0"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="0"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="0"/>
+      <c r="M2" s="0"/>
+      <c r="N2" s="0"/>
       <c r="O2" s="0"/>
       <c r="P2" s="0"/>
       <c r="Q2" s="0"/>
@@ -2552,9 +2523,6 @@
       <c r="AME2" s="0"/>
       <c r="AMF2" s="0"/>
       <c r="AMG2" s="0"/>
-      <c r="AMH2" s="0"/>
-      <c r="AMI2" s="0"/>
-      <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A3" s="0"/>
@@ -2567,15 +2535,15 @@
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="0"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="0"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="0"/>
+      <c r="N3" s="0"/>
+      <c r="O3" s="0"/>
       <c r="P3" s="0"/>
       <c r="Q3" s="0"/>
       <c r="R3" s="0"/>
@@ -3582,9 +3550,6 @@
       <c r="AME3" s="0"/>
       <c r="AMF3" s="0"/>
       <c r="AMG3" s="0"/>
-      <c r="AMH3" s="0"/>
-      <c r="AMI3" s="0"/>
-      <c r="AMJ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0"/>
@@ -4608,9 +4573,6 @@
       <c r="AME4" s="0"/>
       <c r="AMF4" s="0"/>
       <c r="AMG4" s="0"/>
-      <c r="AMH4" s="0"/>
-      <c r="AMI4" s="0"/>
-      <c r="AMJ4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A5" s="0"/>
@@ -4621,15 +4583,15 @@
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="0"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="0"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
       <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
+      <c r="M5" s="0"/>
+      <c r="N5" s="0"/>
+      <c r="O5" s="0"/>
       <c r="P5" s="0"/>
       <c r="Q5" s="0"/>
       <c r="R5" s="0"/>
@@ -5636,9 +5598,6 @@
       <c r="AME5" s="0"/>
       <c r="AMF5" s="0"/>
       <c r="AMG5" s="0"/>
-      <c r="AMH5" s="0"/>
-      <c r="AMI5" s="0"/>
-      <c r="AMJ5" s="0"/>
     </row>
     <row r="6" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B6" s="5"/>
@@ -5652,19 +5611,13 @@
         <v>5</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="AMH6" s="0"/>
+      <c r="AMI6" s="0"/>
+      <c r="AMJ6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A7" s="3"/>
@@ -5673,16 +5626,14 @@
         <v>7</v>
       </c>
       <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="11" t="s">
+      <c r="E7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="1"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="0"/>
+      <c r="I7" s="0"/>
+      <c r="J7" s="0"/>
       <c r="K7" s="0"/>
       <c r="L7" s="0"/>
       <c r="M7" s="0"/>
@@ -6694,63 +6645,48 @@
       <c r="AME7" s="0"/>
       <c r="AMF7" s="0"/>
       <c r="AMG7" s="0"/>
-      <c r="AMH7" s="0"/>
-      <c r="AMI7" s="0"/>
-      <c r="AMJ7" s="0"/>
     </row>
     <row r="8" s="13" customFormat="true" ht="76.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B8" s="14"/>
       <c r="C8" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="E8" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="F8" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="AMH8" s="0"/>
+      <c r="AMI8" s="0"/>
+      <c r="AMJ8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0"/>
       <c r="B9" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="F9" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="I9" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="J9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="0"/>
+      <c r="I9" s="0"/>
+      <c r="J9" s="0"/>
       <c r="K9" s="0"/>
       <c r="L9" s="0"/>
       <c r="M9" s="0"/>
@@ -7762,29 +7698,26 @@
       <c r="AME9" s="0"/>
       <c r="AMF9" s="0"/>
       <c r="AMG9" s="0"/>
-      <c r="AMH9" s="0"/>
-      <c r="AMI9" s="0"/>
-      <c r="AMJ9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0"/>
       <c r="B10" s="20" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D10" s="21"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22" t="s">
-        <v>26</v>
+      <c r="E10" s="22" t="s">
+        <v>20</v>
       </c>
-      <c r="H10" s="23" t="n">
+      <c r="F10" s="23" t="n">
         <v>400</v>
       </c>
-      <c r="I10" s="23"/>
-      <c r="J10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="0"/>
+      <c r="I10" s="0"/>
+      <c r="J10" s="0"/>
       <c r="K10" s="0"/>
       <c r="L10" s="0"/>
       <c r="M10" s="0"/>
@@ -8796,29 +8729,26 @@
       <c r="AME10" s="0"/>
       <c r="AMF10" s="0"/>
       <c r="AMG10" s="0"/>
-      <c r="AMH10" s="0"/>
-      <c r="AMI10" s="0"/>
-      <c r="AMJ10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0"/>
       <c r="B11" s="22" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22" t="s">
-        <v>26</v>
+      <c r="E11" s="22" t="s">
+        <v>20</v>
       </c>
-      <c r="H11" s="22" t="n">
+      <c r="F11" s="22" t="n">
         <v>800</v>
       </c>
-      <c r="I11" s="22"/>
-      <c r="J11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="0"/>
+      <c r="I11" s="0"/>
+      <c r="J11" s="0"/>
       <c r="K11" s="0"/>
       <c r="L11" s="0"/>
       <c r="M11" s="0"/>
@@ -9830,21 +9760,21 @@
       <c r="AME11" s="0"/>
       <c r="AMF11" s="0"/>
       <c r="AMG11" s="0"/>
-      <c r="AMH11" s="0"/>
-      <c r="AMI11" s="0"/>
-      <c r="AMJ11" s="0"/>
     </row>
     <row r="12" s="22" customFormat="true" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="24"/>
       <c r="B12" s="22" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D12" s="22" t="n">
         <v>6</v>
       </c>
-      <c r="H12" s="22" t="n">
+      <c r="F12" s="22" t="n">
         <v>1000</v>
       </c>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
       <c r="L12" s="24"/>
       <c r="M12" s="24"/>
       <c r="N12" s="24"/>
@@ -10091,20 +10021,9 @@
       <c r="IU12" s="24"/>
       <c r="IV12" s="24"/>
       <c r="IW12" s="24"/>
-      <c r="IX12" s="24"/>
-      <c r="IY12" s="24"/>
-      <c r="IZ12" s="24"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E13" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="AMH12" s="0"/>
+      <c r="AMI12" s="0"/>
+      <c r="AMJ12" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="36.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="37.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -10120,8 +10039,8 @@
     <row r="34" customFormat="false" ht="25.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.15" right="0.140277777777778" top="0.179861111111111" bottom="0.2" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Uploaded 16-Feb-2017 16:08:57 {/bonus-program/src/main/resources/dtables/bonus_program/bonus-program.xlsx}
</commit_message>
<xml_diff>
--- a/bonus-program/src/main/resources/dtables/bonus_program/bonus-program.xlsx
+++ b/bonus-program/src/main/resources/dtables/bonus_program/bonus-program.xlsx
@@ -12,7 +12,7 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="ClaimTypes" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" name="Excel_BuiltIn__FilterDatabase_1" vbProcedure="false">Tables!$E$10:$E$21</definedName>
+    <definedName function="false" hidden="false" name="Excel_BuiltIn__FilterDatabase_1" vbProcedure="false">Tables!$G$10:$G$21</definedName>
     <definedName function="false" hidden="false" name="Excel_BuiltIn__FilterDatabase_2" vbProcedure="false">#REF!</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -116,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t>RuleSet</t>
   </si>
@@ -142,6 +142,9 @@
     <t>$e : Employee</t>
   </si>
   <si>
+    <t>$bonus : Bonus</t>
+  </si>
+  <si>
     <t>not Bonus</t>
   </si>
   <si>
@@ -151,10 +154,16 @@
     <t>yearsOfService &gt; $param</t>
   </si>
   <si>
+    <t>bigAbsence == $param</t>
+  </si>
+  <si>
     <t>employee == $param</t>
   </si>
   <si>
     <t>Bonus $b = new Bonus(); $b.setAmount((double)$param); $b.setEmployee($e); insert($b);</t>
+  </si>
+  <si>
+    <t>retract($param)</t>
   </si>
   <si>
     <t>Bonus rules</t>
@@ -166,10 +175,19 @@
     <t>Served more</t>
   </si>
   <si>
+    <t>absence</t>
+  </si>
+  <si>
+    <t>bonus for employee</t>
+  </si>
+  <si>
     <t>no bonus for employee</t>
   </si>
   <si>
     <t>Inser bonus of amount</t>
+  </si>
+  <si>
+    <t>retract</t>
   </si>
   <si>
     <t>Lowest bonus</t>
@@ -189,14 +207,18 @@
   <si>
     <t>High bonus</t>
   </si>
+  <si>
+    <t>$bonus</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -332,7 +354,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -433,6 +455,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -454,7 +480,7 @@
   <dimension ref="1:34"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -462,16 +488,16 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="0.13265306122449"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.8112244897959"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="30.6428571428571"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="1021" min="13" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="4" style="1" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="1" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -482,9 +508,9 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
-      <c r="H1" s="0"/>
-      <c r="I1" s="0"/>
-      <c r="J1" s="0"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
       <c r="K1" s="0"/>
       <c r="L1" s="0"/>
       <c r="M1" s="0"/>
@@ -1496,6 +1522,9 @@
       <c r="AME1" s="0"/>
       <c r="AMF1" s="0"/>
       <c r="AMG1" s="0"/>
+      <c r="AMH1" s="0"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A2" s="0"/>
@@ -1508,14 +1537,14 @@
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="0"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="0"/>
-      <c r="M2" s="0"/>
-      <c r="N2" s="0"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="0"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
       <c r="O2" s="0"/>
       <c r="P2" s="0"/>
       <c r="Q2" s="0"/>
@@ -2523,6 +2552,9 @@
       <c r="AME2" s="0"/>
       <c r="AMF2" s="0"/>
       <c r="AMG2" s="0"/>
+      <c r="AMH2" s="0"/>
+      <c r="AMI2" s="0"/>
+      <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A3" s="0"/>
@@ -2535,15 +2567,15 @@
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="0"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="0"/>
-      <c r="N3" s="0"/>
-      <c r="O3" s="0"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="0"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
       <c r="P3" s="0"/>
       <c r="Q3" s="0"/>
       <c r="R3" s="0"/>
@@ -3550,6 +3582,9 @@
       <c r="AME3" s="0"/>
       <c r="AMF3" s="0"/>
       <c r="AMG3" s="0"/>
+      <c r="AMH3" s="0"/>
+      <c r="AMI3" s="0"/>
+      <c r="AMJ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0"/>
@@ -4573,6 +4608,9 @@
       <c r="AME4" s="0"/>
       <c r="AMF4" s="0"/>
       <c r="AMG4" s="0"/>
+      <c r="AMH4" s="0"/>
+      <c r="AMI4" s="0"/>
+      <c r="AMJ4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A5" s="0"/>
@@ -4583,15 +4621,15 @@
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="0"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="0"/>
       <c r="L5" s="4"/>
-      <c r="M5" s="0"/>
-      <c r="N5" s="0"/>
-      <c r="O5" s="0"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
       <c r="P5" s="0"/>
       <c r="Q5" s="0"/>
       <c r="R5" s="0"/>
@@ -5598,6 +5636,9 @@
       <c r="AME5" s="0"/>
       <c r="AMF5" s="0"/>
       <c r="AMG5" s="0"/>
+      <c r="AMH5" s="0"/>
+      <c r="AMI5" s="0"/>
+      <c r="AMJ5" s="0"/>
     </row>
     <row r="6" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B6" s="5"/>
@@ -5611,13 +5652,19 @@
         <v>5</v>
       </c>
       <c r="F6" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="AMH6" s="0"/>
-      <c r="AMI6" s="0"/>
-      <c r="AMJ6" s="0"/>
+      <c r="I6" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A7" s="3"/>
@@ -5626,14 +5673,16 @@
         <v>7</v>
       </c>
       <c r="D7" s="12"/>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="12"/>
+      <c r="F7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="12"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="0"/>
-      <c r="I7" s="0"/>
-      <c r="J7" s="0"/>
+      <c r="G7" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="1"/>
       <c r="K7" s="0"/>
       <c r="L7" s="0"/>
       <c r="M7" s="0"/>
@@ -6645,48 +6694,63 @@
       <c r="AME7" s="0"/>
       <c r="AMF7" s="0"/>
       <c r="AMG7" s="0"/>
+      <c r="AMH7" s="0"/>
+      <c r="AMI7" s="0"/>
+      <c r="AMJ7" s="0"/>
     </row>
     <row r="8" s="13" customFormat="true" ht="76.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B8" s="14"/>
       <c r="C8" s="15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="AMH8" s="0"/>
-      <c r="AMI8" s="0"/>
-      <c r="AMJ8" s="0"/>
+      <c r="G8" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0"/>
       <c r="B9" s="17" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
-      <c r="F9" s="19" t="s">
-        <v>17</v>
+      <c r="F9" s="18" t="s">
+        <v>20</v>
       </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="0"/>
-      <c r="I9" s="0"/>
-      <c r="J9" s="0"/>
+      <c r="G9" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" s="1"/>
       <c r="K9" s="0"/>
       <c r="L9" s="0"/>
       <c r="M9" s="0"/>
@@ -7698,26 +7762,29 @@
       <c r="AME9" s="0"/>
       <c r="AMF9" s="0"/>
       <c r="AMG9" s="0"/>
+      <c r="AMH9" s="0"/>
+      <c r="AMI9" s="0"/>
+      <c r="AMJ9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0"/>
       <c r="B10" s="20" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D10" s="21"/>
-      <c r="E10" s="22" t="s">
-        <v>20</v>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22" t="s">
+        <v>26</v>
       </c>
-      <c r="F10" s="23" t="n">
+      <c r="H10" s="23" t="n">
         <v>400</v>
       </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="0"/>
-      <c r="I10" s="0"/>
-      <c r="J10" s="0"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="1"/>
       <c r="K10" s="0"/>
       <c r="L10" s="0"/>
       <c r="M10" s="0"/>
@@ -8729,26 +8796,29 @@
       <c r="AME10" s="0"/>
       <c r="AMF10" s="0"/>
       <c r="AMG10" s="0"/>
+      <c r="AMH10" s="0"/>
+      <c r="AMI10" s="0"/>
+      <c r="AMJ10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0"/>
       <c r="B11" s="22" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D11" s="22"/>
-      <c r="E11" s="22" t="s">
-        <v>20</v>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22" t="s">
+        <v>26</v>
       </c>
-      <c r="F11" s="22" t="n">
+      <c r="H11" s="22" t="n">
         <v>800</v>
       </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="0"/>
-      <c r="I11" s="0"/>
-      <c r="J11" s="0"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="1"/>
       <c r="K11" s="0"/>
       <c r="L11" s="0"/>
       <c r="M11" s="0"/>
@@ -9760,21 +9830,21 @@
       <c r="AME11" s="0"/>
       <c r="AMF11" s="0"/>
       <c r="AMG11" s="0"/>
+      <c r="AMH11" s="0"/>
+      <c r="AMI11" s="0"/>
+      <c r="AMJ11" s="0"/>
     </row>
     <row r="12" s="22" customFormat="true" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="24"/>
       <c r="B12" s="22" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D12" s="22" t="n">
         <v>6</v>
       </c>
-      <c r="F12" s="22" t="n">
+      <c r="H12" s="22" t="n">
         <v>1000</v>
       </c>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="24"/>
       <c r="L12" s="24"/>
       <c r="M12" s="24"/>
       <c r="N12" s="24"/>
@@ -10021,9 +10091,20 @@
       <c r="IU12" s="24"/>
       <c r="IV12" s="24"/>
       <c r="IW12" s="24"/>
-      <c r="AMH12" s="0"/>
-      <c r="AMI12" s="0"/>
-      <c r="AMJ12" s="0"/>
+      <c r="IX12" s="24"/>
+      <c r="IY12" s="24"/>
+      <c r="IZ12" s="24"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E13" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="36.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="37.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -10039,8 +10120,8 @@
     <row r="34" customFormat="false" ht="25.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="C7:E7"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.15" right="0.140277777777778" top="0.179861111111111" bottom="0.2" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Uploaded 16-Feb-2017 16:10:07 {/bonus-program/src/main/resources/dtables/bonus_program/bonus-program.xlsx}
</commit_message>
<xml_diff>
--- a/bonus-program/src/main/resources/dtables/bonus_program/bonus-program.xlsx
+++ b/bonus-program/src/main/resources/dtables/bonus_program/bonus-program.xlsx
@@ -116,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>RuleSet</t>
   </si>
@@ -206,6 +206,9 @@
   </si>
   <si>
     <t>High bonus</t>
+  </si>
+  <si>
+    <t>hhh</t>
   </si>
   <si>
     <t>$bonus</t>
@@ -480,24 +483,24 @@
   <dimension ref="1:34"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="0.13265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="7" min="4" style="1" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="30.6428571428571"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="7" min="4" style="1" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="1" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10096,14 +10099,18 @@
       <c r="IZ12" s="24"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E13" s="25" t="b">
+      <c r="B13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="25" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>26</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="36.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Uploaded 16-Feb-2017 16:13:35 {/bonus-program/src/main/resources/dtables/bonus_program/bonus-program.xlsx}
</commit_message>
<xml_diff>
--- a/bonus-program/src/main/resources/dtables/bonus_program/bonus-program.xlsx
+++ b/bonus-program/src/main/resources/dtables/bonus_program/bonus-program.xlsx
@@ -163,7 +163,7 @@
     <t>Bonus $b = new Bonus(); $b.setAmount((double)$param); $b.setEmployee($e); insert($b);</t>
   </si>
   <si>
-    <t>retract($param)</t>
+    <t>retract($param);</t>
   </si>
   <si>
     <t>Bonus rules</t>
@@ -208,7 +208,7 @@
     <t>High bonus</t>
   </si>
   <si>
-    <t>hhh</t>
+    <t>Big absence</t>
   </si>
   <si>
     <t>$bonus</t>
@@ -483,7 +483,7 @@
   <dimension ref="1:34"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -10099,7 +10099,7 @@
       <c r="IZ12" s="24"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E13" s="25" t="n">

</xml_diff>

<commit_message>
Uploaded 16-Feb-2017 16:17:24 {/bonus-program/src/main/resources/dtables/bonus_program/bonus-program.xlsx}
</commit_message>
<xml_diff>
--- a/bonus-program/src/main/resources/dtables/bonus_program/bonus-program.xlsx
+++ b/bonus-program/src/main/resources/dtables/bonus_program/bonus-program.xlsx
@@ -116,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t>RuleSet</t>
   </si>
@@ -148,7 +148,7 @@
     <t>not Bonus</t>
   </si>
   <si>
-    <t>yearsOfService &gt;= $1, yearsOfService &lt; $2</t>
+    <t>YearsOfService &gt;= $1</t>
   </si>
   <si>
     <t>yearsOfService &gt; $param</t>
@@ -193,16 +193,10 @@
     <t>Lowest bonus</t>
   </si>
   <si>
-    <t>0, 2</t>
-  </si>
-  <si>
     <t>$e</t>
   </si>
   <si>
     <t>Middle bonus</t>
-  </si>
-  <si>
-    <t>2, 6</t>
   </si>
   <si>
     <t>High bonus</t>
@@ -483,7 +477,7 @@
   <dimension ref="1:34"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -7774,14 +7768,14 @@
       <c r="B10" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="21" t="s">
-        <v>25</v>
+      <c r="C10" s="21" t="n">
+        <v>0</v>
       </c>
       <c r="D10" s="21"/>
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
       <c r="G10" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H10" s="23" t="n">
         <v>400</v>
@@ -8806,16 +8800,16 @@
     <row r="11" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0"/>
       <c r="B11" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
-      <c r="C11" s="22" t="s">
-        <v>28</v>
+      <c r="C11" s="22" t="n">
+        <v>2</v>
       </c>
       <c r="D11" s="22"/>
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
       <c r="G11" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H11" s="22" t="n">
         <v>800</v>
@@ -9840,7 +9834,7 @@
     <row r="12" s="22" customFormat="true" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="24"/>
       <c r="B12" s="22" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D12" s="22" t="n">
         <v>6</v>
@@ -10100,17 +10094,17 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E13" s="25" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="36.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>